<commit_message>
product ranking record files
</commit_message>
<xml_diff>
--- a/product_ranking_camellia_eyelash_extension.xlsx
+++ b/product_ranking_camellia_eyelash_extension.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\python\Market Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Market Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,14 +20,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
-  <si>
-    <t>2018-10-14 22:53:16</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+  <si>
+    <t>2018-10-15 10:04:53</t>
+  </si>
+  <si>
+    <t>2018-10-15 09:43:23</t>
   </si>
   <si>
     <t>2018-10-14 13:15:58</t>
   </si>
   <si>
+    <t>professional rapid lash camellia eyelash extension mixed length easy fan blooming camelia lash camellia lash</t>
+  </si>
+  <si>
+    <t>professional camellia eyelash extension mixed length easy fan blooming camelia lash camellia lash</t>
+  </si>
+  <si>
     <t>Vegan Easy Fan Volume Blooming Camellia Eyelash Extension</t>
   </si>
   <si>
@@ -37,6 +46,9 @@
     <t>Vegan Easy Fan Volume Blooming Camellia Lash</t>
   </si>
   <si>
+    <t>camellia eyelash extensions</t>
+  </si>
+  <si>
     <t>Vegan Easy Fan Volume Blooming Eyelash Extension Camellia</t>
   </si>
   <si>
@@ -49,15 +61,15 @@
     <t>camellia lashes</t>
   </si>
   <si>
+    <t>1-20</t>
+  </si>
+  <si>
     <t>1-21</t>
   </si>
   <si>
     <t>4-15</t>
   </si>
   <si>
-    <t>camellia eyelash extensions</t>
-  </si>
-  <si>
     <t>12-29</t>
   </si>
   <si>
@@ -67,19 +79,19 @@
     <t>camellia eyelash</t>
   </si>
   <si>
-    <t>4-21</t>
-  </si>
-  <si>
     <t>4-26</t>
   </si>
   <si>
+    <t>4-23</t>
+  </si>
+  <si>
     <t>1-2</t>
   </si>
   <si>
     <t>eyelash extension camellia</t>
   </si>
   <si>
-    <t>3-6</t>
+    <t>3-5</t>
   </si>
   <si>
     <t>3-7</t>
@@ -88,26 +100,25 @@
     <t>mixed length eyelash extension</t>
   </si>
   <si>
-    <t>14-3</t>
+    <t>14-4</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>2-18</t>
+    <t>2-20</t>
   </si>
   <si>
     <t>lash camellia</t>
   </si>
   <si>
-    <t>3-16</t>
+    <t>3-20</t>
+  </si>
+  <si>
+    <t>3-17</t>
   </si>
   <si>
     <t>3-15</t>
-  </si>
-  <si>
-    <t>professional camellia eyelash extension mixed length easy fan blooming camelia lash camellia lash</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>camellia eyelash extensions</t>
@@ -115,10 +126,6 @@
   </si>
   <si>
     <t>camellia eyelash extensions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>camellia eyelash</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -126,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,29 +680,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF59"/>
+  <dimension ref="A1:AG59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="3" width="4.625" style="29" customWidth="1"/>
-    <col min="4" max="10" width="30.625" style="14" customWidth="1"/>
-    <col min="11" max="11" width="30.625" style="40" customWidth="1"/>
-    <col min="12" max="12" width="30.625" style="14" customWidth="1"/>
-    <col min="13" max="22" width="30.625" style="28" customWidth="1"/>
-    <col min="23" max="23" width="30.625" style="2" customWidth="1"/>
-    <col min="24" max="24" width="30.625" style="28" customWidth="1"/>
-    <col min="25" max="28" width="31" style="28" customWidth="1"/>
-    <col min="29" max="29" width="31" style="7" customWidth="1"/>
-    <col min="30" max="30" width="41.625" style="3" customWidth="1"/>
-    <col min="31" max="31" width="45.75" style="3" customWidth="1"/>
-    <col min="32" max="32" width="40.625" style="45" customWidth="1"/>
+    <col min="4" max="11" width="30.625" style="14" customWidth="1"/>
+    <col min="12" max="12" width="30.625" style="40" customWidth="1"/>
+    <col min="13" max="13" width="30.625" style="14" customWidth="1"/>
+    <col min="14" max="23" width="30.625" style="28" customWidth="1"/>
+    <col min="24" max="24" width="30.625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="30.625" style="28" customWidth="1"/>
+    <col min="26" max="29" width="31" style="28" customWidth="1"/>
+    <col min="30" max="30" width="31" style="7" customWidth="1"/>
+    <col min="31" max="31" width="41.625" style="3" customWidth="1"/>
+    <col min="32" max="32" width="45.75" style="3" customWidth="1"/>
+    <col min="33" max="33" width="40.625" style="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="1" customFormat="1">
       <c r="A1" s="29"/>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -705,7 +712,9 @@
       <c r="F1" s="1">
         <v>60764339320</v>
       </c>
-      <c r="J1" s="45"/>
+      <c r="G1" s="1">
+        <v>60764339320</v>
+      </c>
       <c r="K1" s="45"/>
       <c r="L1" s="45"/>
       <c r="M1" s="45"/>
@@ -720,15 +729,16 @@
       <c r="V1" s="45"/>
       <c r="W1" s="45"/>
       <c r="X1" s="45"/>
-      <c r="Z1" s="45"/>
+      <c r="Y1" s="45"/>
       <c r="AA1" s="45"/>
       <c r="AB1" s="45"/>
       <c r="AC1" s="45"/>
       <c r="AD1" s="45"/>
       <c r="AE1" s="45"/>
       <c r="AF1" s="45"/>
-    </row>
-    <row r="2" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG1" s="45"/>
+    </row>
+    <row r="2" spans="1:33" s="22" customFormat="1">
       <c r="A2" s="30"/>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -739,12 +749,14 @@
       <c r="F2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="31"/>
+      <c r="G2" s="31" t="s">
+        <v>2</v>
+      </c>
       <c r="H2" s="31"/>
       <c r="I2" s="31"/>
       <c r="J2" s="31"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="18"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="38"/>
       <c r="M2" s="18"/>
       <c r="N2" s="18"/>
       <c r="O2" s="18"/>
@@ -754,33 +766,36 @@
       <c r="S2" s="18"/>
       <c r="T2" s="18"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="23"/>
+      <c r="V2" s="18"/>
       <c r="W2" s="23"/>
       <c r="X2" s="23"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="19"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="18"/>
       <c r="AA2" s="19"/>
-      <c r="AB2" s="20"/>
+      <c r="AB2" s="19"/>
       <c r="AC2" s="20"/>
-      <c r="AD2" s="21"/>
-      <c r="AE2" s="23"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="21"/>
       <c r="AF2" s="23"/>
-    </row>
-    <row r="3" spans="1:32" s="11" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG2" s="23"/>
+    </row>
+    <row r="3" spans="1:33" s="11" customFormat="1" ht="63" customHeight="1">
       <c r="A3" s="29"/>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
       <c r="D3" s="32">
-        <f>LEN(E3)</f>
+        <f>LEN(F3)</f>
         <v>97</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="32"/>
+        <v>4</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>5</v>
+      </c>
       <c r="H3" s="32"/>
       <c r="I3" s="32"/>
       <c r="J3" s="32"/>
@@ -789,41 +804,44 @@
       <c r="M3" s="32"/>
       <c r="N3" s="32"/>
       <c r="O3" s="32"/>
-      <c r="P3" s="10"/>
+      <c r="P3" s="32"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="32"/>
-      <c r="Z3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="32"/>
       <c r="AA3" s="10"/>
       <c r="AB3" s="10"/>
       <c r="AC3" s="10"/>
-      <c r="AD3" s="32"/>
+      <c r="AD3" s="10"/>
       <c r="AE3" s="32"/>
       <c r="AF3" s="32"/>
-    </row>
-    <row r="4" spans="1:32" s="11" customFormat="1" ht="54.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG3" s="32"/>
+    </row>
+    <row r="4" spans="1:33" s="11" customFormat="1" ht="54.95" customHeight="1">
       <c r="A4" s="29"/>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
       <c r="D4" s="50"/>
       <c r="E4" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="50"/>
-      <c r="H4" s="41"/>
+        <v>6</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="50"/>
       <c r="I4" s="41"/>
       <c r="J4" s="41"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="32"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="41"/>
       <c r="N4" s="32"/>
       <c r="O4" s="32"/>
       <c r="P4" s="32"/>
@@ -831,36 +849,39 @@
       <c r="R4" s="32"/>
       <c r="S4" s="32"/>
       <c r="T4" s="32"/>
-      <c r="U4" s="50"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="32"/>
-      <c r="Z4" s="10"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="50"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="32"/>
       <c r="AA4" s="10"/>
       <c r="AB4" s="10"/>
       <c r="AC4" s="10"/>
-      <c r="AD4" s="32"/>
+      <c r="AD4" s="10"/>
       <c r="AE4" s="32"/>
       <c r="AF4" s="32"/>
-    </row>
-    <row r="5" spans="1:32" s="11" customFormat="1" ht="54.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG4" s="32"/>
+    </row>
+    <row r="5" spans="1:33" s="11" customFormat="1" ht="54.95" customHeight="1">
       <c r="A5" s="29"/>
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="41"/>
       <c r="E5" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="50" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="31"/>
+        <v>34</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="41"/>
       <c r="I5" s="31"/>
       <c r="J5" s="31"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="32"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="41"/>
       <c r="N5" s="32"/>
       <c r="O5" s="32"/>
       <c r="P5" s="32"/>
@@ -868,36 +889,39 @@
       <c r="R5" s="32"/>
       <c r="S5" s="32"/>
       <c r="T5" s="32"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="32"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="32"/>
-      <c r="Z5" s="10"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="50"/>
+      <c r="W5" s="32"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="32"/>
       <c r="AA5" s="10"/>
       <c r="AB5" s="10"/>
       <c r="AC5" s="10"/>
-      <c r="AD5" s="32"/>
+      <c r="AD5" s="10"/>
       <c r="AE5" s="32"/>
       <c r="AF5" s="32"/>
-    </row>
-    <row r="6" spans="1:32" s="11" customFormat="1" ht="54.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG5" s="32"/>
+    </row>
+    <row r="6" spans="1:33" s="11" customFormat="1" ht="54.95" customHeight="1">
       <c r="A6" s="29"/>
       <c r="B6" s="29"/>
       <c r="C6" s="29"/>
       <c r="D6" s="41"/>
       <c r="E6" s="41" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="41"/>
+        <v>10</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>11</v>
+      </c>
       <c r="H6" s="41"/>
       <c r="I6" s="41"/>
       <c r="J6" s="41"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="32"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="41"/>
       <c r="N6" s="32"/>
       <c r="O6" s="32"/>
       <c r="P6" s="32"/>
@@ -905,19 +929,20 @@
       <c r="R6" s="32"/>
       <c r="S6" s="32"/>
       <c r="T6" s="32"/>
-      <c r="U6" s="50"/>
-      <c r="V6" s="32"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="12"/>
-      <c r="Z6" s="10"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="50"/>
+      <c r="W6" s="32"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="12"/>
       <c r="AA6" s="10"/>
       <c r="AB6" s="10"/>
       <c r="AC6" s="10"/>
-      <c r="AD6" s="32"/>
+      <c r="AD6" s="10"/>
       <c r="AE6" s="32"/>
       <c r="AF6" s="32"/>
-    </row>
-    <row r="7" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG6" s="32"/>
+    </row>
+    <row r="7" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A7">
         <v>66</v>
       </c>
@@ -928,20 +953,22 @@
         <v>134</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="34"/>
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
       <c r="J7" s="34"/>
-      <c r="K7" s="51"/>
+      <c r="K7" s="34"/>
       <c r="L7" s="51"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="44"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="43"/>
       <c r="O7" s="44"/>
       <c r="P7" s="44"/>
       <c r="Q7" s="44"/>
@@ -949,19 +976,20 @@
       <c r="S7" s="44"/>
       <c r="T7" s="44"/>
       <c r="U7" s="44"/>
-      <c r="V7" s="43"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="43"/>
-      <c r="Y7" s="44"/>
+      <c r="V7" s="44"/>
+      <c r="W7" s="43"/>
+      <c r="X7" s="45"/>
+      <c r="Y7" s="43"/>
       <c r="Z7" s="44"/>
-      <c r="AA7" s="46"/>
+      <c r="AA7" s="44"/>
       <c r="AB7" s="46"/>
-      <c r="AC7" s="47"/>
-      <c r="AD7" s="48"/>
+      <c r="AC7" s="46"/>
+      <c r="AD7" s="47"/>
       <c r="AE7" s="48"/>
-      <c r="AF7" s="49"/>
-    </row>
-    <row r="8" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF7" s="48"/>
+      <c r="AG7" s="49"/>
+    </row>
+    <row r="8" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A8">
         <v>59</v>
       </c>
@@ -972,20 +1000,22 @@
         <v>128</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="34"/>
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
       <c r="J8" s="34"/>
-      <c r="K8" s="51"/>
+      <c r="K8" s="34"/>
       <c r="L8" s="51"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="44"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="43"/>
       <c r="O8" s="44"/>
       <c r="P8" s="44"/>
       <c r="Q8" s="44"/>
@@ -993,19 +1023,20 @@
       <c r="S8" s="44"/>
       <c r="T8" s="44"/>
       <c r="U8" s="44"/>
-      <c r="V8" s="43"/>
-      <c r="W8" s="45"/>
-      <c r="X8" s="43"/>
-      <c r="Y8" s="44"/>
+      <c r="V8" s="44"/>
+      <c r="W8" s="43"/>
+      <c r="X8" s="45"/>
+      <c r="Y8" s="43"/>
       <c r="Z8" s="44"/>
-      <c r="AA8" s="46"/>
+      <c r="AA8" s="44"/>
       <c r="AB8" s="46"/>
-      <c r="AC8" s="47"/>
-      <c r="AD8" s="48"/>
+      <c r="AC8" s="46"/>
+      <c r="AD8" s="47"/>
       <c r="AE8" s="48"/>
-      <c r="AF8" s="49"/>
-    </row>
-    <row r="9" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF8" s="48"/>
+      <c r="AG8" s="49"/>
+    </row>
+    <row r="9" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A9">
         <v>37</v>
       </c>
@@ -1016,20 +1047,22 @@
         <v>89</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="35"/>
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
       <c r="J9" s="35"/>
-      <c r="K9" s="51"/>
+      <c r="K9" s="35"/>
       <c r="L9" s="51"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="44"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="43"/>
       <c r="O9" s="44"/>
       <c r="P9" s="44"/>
       <c r="Q9" s="44"/>
@@ -1037,19 +1070,20 @@
       <c r="S9" s="44"/>
       <c r="T9" s="44"/>
       <c r="U9" s="44"/>
-      <c r="V9" s="43"/>
-      <c r="W9" s="45"/>
-      <c r="X9" s="43"/>
-      <c r="Y9" s="44"/>
+      <c r="V9" s="44"/>
+      <c r="W9" s="43"/>
+      <c r="X9" s="45"/>
+      <c r="Y9" s="43"/>
       <c r="Z9" s="44"/>
-      <c r="AA9" s="46"/>
+      <c r="AA9" s="44"/>
       <c r="AB9" s="46"/>
-      <c r="AC9" s="47"/>
-      <c r="AD9" s="48"/>
+      <c r="AC9" s="46"/>
+      <c r="AD9" s="47"/>
       <c r="AE9" s="48"/>
-      <c r="AF9" s="49"/>
-    </row>
-    <row r="10" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF9" s="48"/>
+      <c r="AG9" s="49"/>
+    </row>
+    <row r="10" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1060,17 +1094,19 @@
         <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="35"/>
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
       <c r="J10" s="35"/>
-      <c r="K10" s="51"/>
+      <c r="K10" s="35"/>
       <c r="L10" s="51"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="44"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="43"/>
       <c r="O10" s="44"/>
       <c r="P10" s="44"/>
       <c r="Q10" s="44"/>
@@ -1078,19 +1114,20 @@
       <c r="S10" s="44"/>
       <c r="T10" s="44"/>
       <c r="U10" s="44"/>
-      <c r="V10" s="43"/>
-      <c r="W10" s="45"/>
-      <c r="X10" s="43"/>
-      <c r="Y10" s="44"/>
+      <c r="V10" s="44"/>
+      <c r="W10" s="43"/>
+      <c r="X10" s="45"/>
+      <c r="Y10" s="43"/>
       <c r="Z10" s="44"/>
-      <c r="AA10" s="46"/>
+      <c r="AA10" s="44"/>
       <c r="AB10" s="46"/>
-      <c r="AC10" s="47"/>
-      <c r="AD10" s="48"/>
+      <c r="AC10" s="46"/>
+      <c r="AD10" s="47"/>
       <c r="AE10" s="48"/>
-      <c r="AF10" s="49"/>
-    </row>
-    <row r="11" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF10" s="48"/>
+      <c r="AG10" s="49"/>
+    </row>
+    <row r="11" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1101,20 +1138,22 @@
         <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="35"/>
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
       <c r="J11" s="35"/>
-      <c r="K11" s="51"/>
+      <c r="K11" s="35"/>
       <c r="L11" s="51"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="44"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="43"/>
       <c r="O11" s="44"/>
       <c r="P11" s="44"/>
       <c r="Q11" s="44"/>
@@ -1122,19 +1161,20 @@
       <c r="S11" s="44"/>
       <c r="T11" s="44"/>
       <c r="U11" s="44"/>
-      <c r="V11" s="43"/>
-      <c r="W11" s="45"/>
-      <c r="X11" s="43"/>
-      <c r="Y11" s="44"/>
+      <c r="V11" s="44"/>
+      <c r="W11" s="43"/>
+      <c r="X11" s="45"/>
+      <c r="Y11" s="43"/>
       <c r="Z11" s="44"/>
-      <c r="AA11" s="46"/>
+      <c r="AA11" s="44"/>
       <c r="AB11" s="46"/>
-      <c r="AC11" s="47"/>
-      <c r="AD11" s="48"/>
+      <c r="AC11" s="46"/>
+      <c r="AD11" s="47"/>
       <c r="AE11" s="48"/>
-      <c r="AF11" s="49"/>
-    </row>
-    <row r="12" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF11" s="48"/>
+      <c r="AG11" s="49"/>
+    </row>
+    <row r="12" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A12">
         <v>28</v>
       </c>
@@ -1145,20 +1185,22 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="35"/>
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
       <c r="J12" s="35"/>
-      <c r="K12" s="51"/>
+      <c r="K12" s="35"/>
       <c r="L12" s="51"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="44"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="43"/>
       <c r="O12" s="44"/>
       <c r="P12" s="44"/>
       <c r="Q12" s="44"/>
@@ -1166,19 +1208,20 @@
       <c r="S12" s="44"/>
       <c r="T12" s="44"/>
       <c r="U12" s="44"/>
-      <c r="V12" s="43"/>
-      <c r="W12" s="45"/>
-      <c r="X12" s="43"/>
-      <c r="Y12" s="44"/>
+      <c r="V12" s="44"/>
+      <c r="W12" s="43"/>
+      <c r="X12" s="45"/>
+      <c r="Y12" s="43"/>
       <c r="Z12" s="44"/>
-      <c r="AA12" s="46"/>
+      <c r="AA12" s="44"/>
       <c r="AB12" s="46"/>
-      <c r="AC12" s="47"/>
-      <c r="AD12" s="48"/>
+      <c r="AC12" s="46"/>
+      <c r="AD12" s="47"/>
       <c r="AE12" s="48"/>
-      <c r="AF12" s="49"/>
-    </row>
-    <row r="13" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF12" s="48"/>
+      <c r="AG12" s="49"/>
+    </row>
+    <row r="13" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1189,20 +1232,22 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="35"/>
+        <v>28</v>
+      </c>
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
       <c r="J13" s="35"/>
-      <c r="K13" s="51"/>
+      <c r="K13" s="35"/>
       <c r="L13" s="51"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="44"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="43"/>
       <c r="O13" s="44"/>
       <c r="P13" s="44"/>
       <c r="Q13" s="44"/>
@@ -1210,19 +1255,20 @@
       <c r="S13" s="44"/>
       <c r="T13" s="44"/>
       <c r="U13" s="44"/>
-      <c r="V13" s="43"/>
-      <c r="W13" s="45"/>
-      <c r="X13" s="43"/>
-      <c r="Y13" s="44"/>
+      <c r="V13" s="44"/>
+      <c r="W13" s="43"/>
+      <c r="X13" s="45"/>
+      <c r="Y13" s="43"/>
       <c r="Z13" s="44"/>
-      <c r="AA13" s="46"/>
+      <c r="AA13" s="44"/>
       <c r="AB13" s="46"/>
-      <c r="AC13" s="47"/>
-      <c r="AD13" s="48"/>
+      <c r="AC13" s="46"/>
+      <c r="AD13" s="47"/>
       <c r="AE13" s="48"/>
-      <c r="AF13" s="49"/>
-    </row>
-    <row r="14" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF13" s="48"/>
+      <c r="AG13" s="49"/>
+    </row>
+    <row r="14" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1233,20 +1279,22 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="35"/>
+        <v>31</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
       <c r="J14" s="35"/>
-      <c r="K14" s="51"/>
+      <c r="K14" s="35"/>
       <c r="L14" s="51"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="44"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="43"/>
       <c r="O14" s="44"/>
       <c r="P14" s="44"/>
       <c r="Q14" s="44"/>
@@ -1254,19 +1302,20 @@
       <c r="S14" s="44"/>
       <c r="T14" s="44"/>
       <c r="U14" s="44"/>
-      <c r="V14" s="43"/>
-      <c r="W14" s="45"/>
-      <c r="X14" s="43"/>
-      <c r="Y14" s="44"/>
+      <c r="V14" s="44"/>
+      <c r="W14" s="43"/>
+      <c r="X14" s="45"/>
+      <c r="Y14" s="43"/>
       <c r="Z14" s="44"/>
-      <c r="AA14" s="46"/>
+      <c r="AA14" s="44"/>
       <c r="AB14" s="46"/>
-      <c r="AC14" s="47"/>
-      <c r="AD14" s="48"/>
+      <c r="AC14" s="46"/>
+      <c r="AD14" s="47"/>
       <c r="AE14" s="48"/>
-      <c r="AF14" s="49"/>
-    </row>
-    <row r="15" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF14" s="48"/>
+      <c r="AG14" s="49"/>
+    </row>
+    <row r="15" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="33"/>
       <c r="B15" s="33"/>
       <c r="C15" s="33"/>
@@ -1277,10 +1326,10 @@
       <c r="H15" s="35"/>
       <c r="I15" s="35"/>
       <c r="J15" s="35"/>
-      <c r="K15" s="51"/>
+      <c r="K15" s="35"/>
       <c r="L15" s="51"/>
-      <c r="M15" s="43"/>
-      <c r="N15" s="44"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="43"/>
       <c r="O15" s="44"/>
       <c r="P15" s="44"/>
       <c r="Q15" s="44"/>
@@ -1288,19 +1337,20 @@
       <c r="S15" s="44"/>
       <c r="T15" s="44"/>
       <c r="U15" s="44"/>
-      <c r="V15" s="43"/>
-      <c r="W15" s="45"/>
-      <c r="X15" s="43"/>
-      <c r="Y15" s="44"/>
+      <c r="V15" s="44"/>
+      <c r="W15" s="43"/>
+      <c r="X15" s="45"/>
+      <c r="Y15" s="43"/>
       <c r="Z15" s="44"/>
-      <c r="AA15" s="46"/>
+      <c r="AA15" s="44"/>
       <c r="AB15" s="46"/>
-      <c r="AC15" s="47"/>
-      <c r="AD15" s="48"/>
+      <c r="AC15" s="46"/>
+      <c r="AD15" s="47"/>
       <c r="AE15" s="48"/>
-      <c r="AF15" s="49"/>
-    </row>
-    <row r="16" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF15" s="48"/>
+      <c r="AG15" s="49"/>
+    </row>
+    <row r="16" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="33"/>
       <c r="B16" s="33"/>
       <c r="C16" s="33"/>
@@ -1311,10 +1361,10 @@
       <c r="H16" s="35"/>
       <c r="I16" s="35"/>
       <c r="J16" s="35"/>
-      <c r="K16" s="51"/>
+      <c r="K16" s="35"/>
       <c r="L16" s="51"/>
-      <c r="M16" s="43"/>
-      <c r="N16" s="44"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="43"/>
       <c r="O16" s="44"/>
       <c r="P16" s="44"/>
       <c r="Q16" s="44"/>
@@ -1322,19 +1372,20 @@
       <c r="S16" s="44"/>
       <c r="T16" s="44"/>
       <c r="U16" s="44"/>
-      <c r="V16" s="43"/>
-      <c r="W16" s="45"/>
-      <c r="X16" s="43"/>
-      <c r="Y16" s="44"/>
+      <c r="V16" s="44"/>
+      <c r="W16" s="43"/>
+      <c r="X16" s="45"/>
+      <c r="Y16" s="43"/>
       <c r="Z16" s="44"/>
-      <c r="AA16" s="46"/>
+      <c r="AA16" s="44"/>
       <c r="AB16" s="46"/>
-      <c r="AC16" s="47"/>
-      <c r="AD16" s="48"/>
+      <c r="AC16" s="46"/>
+      <c r="AD16" s="47"/>
       <c r="AE16" s="48"/>
-      <c r="AF16" s="49"/>
-    </row>
-    <row r="17" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF16" s="48"/>
+      <c r="AG16" s="49"/>
+    </row>
+    <row r="17" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="33"/>
       <c r="B17" s="33"/>
       <c r="C17" s="33"/>
@@ -1345,10 +1396,10 @@
       <c r="H17" s="35"/>
       <c r="I17" s="35"/>
       <c r="J17" s="35"/>
-      <c r="K17" s="51"/>
+      <c r="K17" s="35"/>
       <c r="L17" s="51"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="44"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="43"/>
       <c r="O17" s="44"/>
       <c r="P17" s="44"/>
       <c r="Q17" s="44"/>
@@ -1356,19 +1407,20 @@
       <c r="S17" s="44"/>
       <c r="T17" s="44"/>
       <c r="U17" s="44"/>
-      <c r="V17" s="43"/>
-      <c r="W17" s="45"/>
-      <c r="X17" s="43"/>
-      <c r="Y17" s="44"/>
+      <c r="V17" s="44"/>
+      <c r="W17" s="43"/>
+      <c r="X17" s="45"/>
+      <c r="Y17" s="43"/>
       <c r="Z17" s="44"/>
-      <c r="AA17" s="46"/>
+      <c r="AA17" s="44"/>
       <c r="AB17" s="46"/>
-      <c r="AC17" s="47"/>
-      <c r="AD17" s="48"/>
+      <c r="AC17" s="46"/>
+      <c r="AD17" s="47"/>
       <c r="AE17" s="48"/>
-      <c r="AF17" s="49"/>
-    </row>
-    <row r="18" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF17" s="48"/>
+      <c r="AG17" s="49"/>
+    </row>
+    <row r="18" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="33"/>
       <c r="B18" s="33"/>
       <c r="C18" s="33"/>
@@ -1379,10 +1431,10 @@
       <c r="H18" s="35"/>
       <c r="I18" s="35"/>
       <c r="J18" s="35"/>
-      <c r="K18" s="51"/>
+      <c r="K18" s="35"/>
       <c r="L18" s="51"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="44"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="43"/>
       <c r="O18" s="44"/>
       <c r="P18" s="44"/>
       <c r="Q18" s="44"/>
@@ -1390,19 +1442,20 @@
       <c r="S18" s="44"/>
       <c r="T18" s="44"/>
       <c r="U18" s="44"/>
-      <c r="V18" s="43"/>
-      <c r="W18" s="45"/>
-      <c r="X18" s="43"/>
-      <c r="Y18" s="44"/>
+      <c r="V18" s="44"/>
+      <c r="W18" s="43"/>
+      <c r="X18" s="45"/>
+      <c r="Y18" s="43"/>
       <c r="Z18" s="44"/>
-      <c r="AA18" s="46"/>
+      <c r="AA18" s="44"/>
       <c r="AB18" s="46"/>
-      <c r="AC18" s="47"/>
-      <c r="AD18" s="48"/>
+      <c r="AC18" s="46"/>
+      <c r="AD18" s="47"/>
       <c r="AE18" s="48"/>
-      <c r="AF18" s="49"/>
-    </row>
-    <row r="19" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF18" s="48"/>
+      <c r="AG18" s="49"/>
+    </row>
+    <row r="19" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A19" s="33"/>
       <c r="B19" s="33"/>
       <c r="C19" s="33"/>
@@ -1413,10 +1466,10 @@
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
       <c r="J19" s="35"/>
-      <c r="K19" s="51"/>
+      <c r="K19" s="35"/>
       <c r="L19" s="51"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="44"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="43"/>
       <c r="O19" s="44"/>
       <c r="P19" s="44"/>
       <c r="Q19" s="44"/>
@@ -1424,19 +1477,20 @@
       <c r="S19" s="44"/>
       <c r="T19" s="44"/>
       <c r="U19" s="44"/>
-      <c r="V19" s="43"/>
-      <c r="W19" s="45"/>
-      <c r="X19" s="43"/>
-      <c r="Y19" s="44"/>
+      <c r="V19" s="44"/>
+      <c r="W19" s="43"/>
+      <c r="X19" s="45"/>
+      <c r="Y19" s="43"/>
       <c r="Z19" s="44"/>
-      <c r="AA19" s="46"/>
+      <c r="AA19" s="44"/>
       <c r="AB19" s="46"/>
-      <c r="AC19" s="47"/>
-      <c r="AD19" s="48"/>
+      <c r="AC19" s="46"/>
+      <c r="AD19" s="47"/>
       <c r="AE19" s="48"/>
-      <c r="AF19" s="49"/>
-    </row>
-    <row r="20" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF19" s="48"/>
+      <c r="AG19" s="49"/>
+    </row>
+    <row r="20" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A20" s="33"/>
       <c r="B20" s="33"/>
       <c r="C20" s="33"/>
@@ -1447,10 +1501,10 @@
       <c r="H20" s="35"/>
       <c r="I20" s="35"/>
       <c r="J20" s="35"/>
-      <c r="K20" s="51"/>
+      <c r="K20" s="35"/>
       <c r="L20" s="51"/>
-      <c r="M20" s="43"/>
-      <c r="N20" s="44"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="43"/>
       <c r="O20" s="44"/>
       <c r="P20" s="44"/>
       <c r="Q20" s="44"/>
@@ -1458,19 +1512,20 @@
       <c r="S20" s="44"/>
       <c r="T20" s="44"/>
       <c r="U20" s="44"/>
-      <c r="V20" s="43"/>
-      <c r="W20" s="45"/>
-      <c r="X20" s="43"/>
-      <c r="Y20" s="44"/>
+      <c r="V20" s="44"/>
+      <c r="W20" s="43"/>
+      <c r="X20" s="45"/>
+      <c r="Y20" s="43"/>
       <c r="Z20" s="44"/>
-      <c r="AA20" s="46"/>
+      <c r="AA20" s="44"/>
       <c r="AB20" s="46"/>
-      <c r="AC20" s="47"/>
-      <c r="AD20" s="48"/>
+      <c r="AC20" s="46"/>
+      <c r="AD20" s="47"/>
       <c r="AE20" s="48"/>
-      <c r="AF20" s="49"/>
-    </row>
-    <row r="21" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF20" s="48"/>
+      <c r="AG20" s="49"/>
+    </row>
+    <row r="21" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A21" s="33"/>
       <c r="B21" s="33"/>
       <c r="C21" s="33"/>
@@ -1481,10 +1536,10 @@
       <c r="H21" s="35"/>
       <c r="I21" s="35"/>
       <c r="J21" s="35"/>
-      <c r="K21" s="51"/>
+      <c r="K21" s="35"/>
       <c r="L21" s="51"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="44"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="43"/>
       <c r="O21" s="44"/>
       <c r="P21" s="44"/>
       <c r="Q21" s="44"/>
@@ -1492,19 +1547,20 @@
       <c r="S21" s="44"/>
       <c r="T21" s="44"/>
       <c r="U21" s="44"/>
-      <c r="V21" s="43"/>
-      <c r="W21" s="45"/>
-      <c r="X21" s="43"/>
-      <c r="Y21" s="44"/>
+      <c r="V21" s="44"/>
+      <c r="W21" s="43"/>
+      <c r="X21" s="45"/>
+      <c r="Y21" s="43"/>
       <c r="Z21" s="44"/>
-      <c r="AA21" s="46"/>
+      <c r="AA21" s="44"/>
       <c r="AB21" s="46"/>
-      <c r="AC21" s="47"/>
-      <c r="AD21" s="48"/>
+      <c r="AC21" s="46"/>
+      <c r="AD21" s="47"/>
       <c r="AE21" s="48"/>
-      <c r="AF21" s="49"/>
-    </row>
-    <row r="22" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF21" s="48"/>
+      <c r="AG21" s="49"/>
+    </row>
+    <row r="22" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A22" s="33"/>
       <c r="B22" s="33"/>
       <c r="C22" s="33"/>
@@ -1515,10 +1571,10 @@
       <c r="H22" s="35"/>
       <c r="I22" s="35"/>
       <c r="J22" s="35"/>
-      <c r="K22" s="51"/>
+      <c r="K22" s="35"/>
       <c r="L22" s="51"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="44"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="43"/>
       <c r="O22" s="44"/>
       <c r="P22" s="44"/>
       <c r="Q22" s="44"/>
@@ -1526,19 +1582,20 @@
       <c r="S22" s="44"/>
       <c r="T22" s="44"/>
       <c r="U22" s="44"/>
-      <c r="V22" s="43"/>
-      <c r="W22" s="45"/>
-      <c r="X22" s="43"/>
-      <c r="Y22" s="44"/>
+      <c r="V22" s="44"/>
+      <c r="W22" s="43"/>
+      <c r="X22" s="45"/>
+      <c r="Y22" s="43"/>
       <c r="Z22" s="44"/>
-      <c r="AA22" s="46"/>
+      <c r="AA22" s="44"/>
       <c r="AB22" s="46"/>
-      <c r="AC22" s="47"/>
-      <c r="AD22" s="48"/>
+      <c r="AC22" s="46"/>
+      <c r="AD22" s="47"/>
       <c r="AE22" s="48"/>
-      <c r="AF22" s="49"/>
-    </row>
-    <row r="23" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF22" s="48"/>
+      <c r="AG22" s="49"/>
+    </row>
+    <row r="23" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A23" s="33"/>
       <c r="B23" s="33"/>
       <c r="C23" s="33"/>
@@ -1549,10 +1606,10 @@
       <c r="H23" s="35"/>
       <c r="I23" s="35"/>
       <c r="J23" s="35"/>
-      <c r="K23" s="51"/>
+      <c r="K23" s="35"/>
       <c r="L23" s="51"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="44"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="43"/>
       <c r="O23" s="44"/>
       <c r="P23" s="44"/>
       <c r="Q23" s="44"/>
@@ -1560,19 +1617,20 @@
       <c r="S23" s="44"/>
       <c r="T23" s="44"/>
       <c r="U23" s="44"/>
-      <c r="V23" s="43"/>
-      <c r="W23" s="45"/>
-      <c r="X23" s="43"/>
-      <c r="Y23" s="44"/>
+      <c r="V23" s="44"/>
+      <c r="W23" s="43"/>
+      <c r="X23" s="45"/>
+      <c r="Y23" s="43"/>
       <c r="Z23" s="44"/>
-      <c r="AA23" s="46"/>
+      <c r="AA23" s="44"/>
       <c r="AB23" s="46"/>
-      <c r="AC23" s="47"/>
-      <c r="AD23" s="48"/>
+      <c r="AC23" s="46"/>
+      <c r="AD23" s="47"/>
       <c r="AE23" s="48"/>
-      <c r="AF23" s="49"/>
-    </row>
-    <row r="24" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF23" s="48"/>
+      <c r="AG23" s="49"/>
+    </row>
+    <row r="24" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A24" s="33"/>
       <c r="B24" s="33"/>
       <c r="C24" s="33"/>
@@ -1583,10 +1641,10 @@
       <c r="H24" s="35"/>
       <c r="I24" s="35"/>
       <c r="J24" s="35"/>
-      <c r="K24" s="51"/>
+      <c r="K24" s="35"/>
       <c r="L24" s="51"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="44"/>
+      <c r="M24" s="51"/>
+      <c r="N24" s="43"/>
       <c r="O24" s="44"/>
       <c r="P24" s="44"/>
       <c r="Q24" s="44"/>
@@ -1594,19 +1652,20 @@
       <c r="S24" s="44"/>
       <c r="T24" s="44"/>
       <c r="U24" s="44"/>
-      <c r="V24" s="43"/>
-      <c r="W24" s="45"/>
-      <c r="X24" s="43"/>
-      <c r="Y24" s="44"/>
+      <c r="V24" s="44"/>
+      <c r="W24" s="43"/>
+      <c r="X24" s="45"/>
+      <c r="Y24" s="43"/>
       <c r="Z24" s="44"/>
-      <c r="AA24" s="46"/>
+      <c r="AA24" s="44"/>
       <c r="AB24" s="46"/>
-      <c r="AC24" s="47"/>
-      <c r="AD24" s="48"/>
+      <c r="AC24" s="46"/>
+      <c r="AD24" s="47"/>
       <c r="AE24" s="48"/>
-      <c r="AF24" s="49"/>
-    </row>
-    <row r="25" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF24" s="48"/>
+      <c r="AG24" s="49"/>
+    </row>
+    <row r="25" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A25" s="33"/>
       <c r="B25" s="33"/>
       <c r="C25" s="33"/>
@@ -1617,10 +1676,10 @@
       <c r="H25" s="35"/>
       <c r="I25" s="35"/>
       <c r="J25" s="35"/>
-      <c r="K25" s="51"/>
+      <c r="K25" s="35"/>
       <c r="L25" s="51"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="44"/>
+      <c r="M25" s="51"/>
+      <c r="N25" s="43"/>
       <c r="O25" s="44"/>
       <c r="P25" s="44"/>
       <c r="Q25" s="44"/>
@@ -1628,19 +1687,20 @@
       <c r="S25" s="44"/>
       <c r="T25" s="44"/>
       <c r="U25" s="44"/>
-      <c r="V25" s="43"/>
-      <c r="W25" s="45"/>
-      <c r="X25" s="43"/>
-      <c r="Y25" s="44"/>
+      <c r="V25" s="44"/>
+      <c r="W25" s="43"/>
+      <c r="X25" s="45"/>
+      <c r="Y25" s="43"/>
       <c r="Z25" s="44"/>
-      <c r="AA25" s="46"/>
+      <c r="AA25" s="44"/>
       <c r="AB25" s="46"/>
-      <c r="AC25" s="47"/>
-      <c r="AD25" s="48"/>
+      <c r="AC25" s="46"/>
+      <c r="AD25" s="47"/>
       <c r="AE25" s="48"/>
-      <c r="AF25" s="49"/>
-    </row>
-    <row r="26" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF25" s="48"/>
+      <c r="AG25" s="49"/>
+    </row>
+    <row r="26" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A26" s="33"/>
       <c r="B26" s="33"/>
       <c r="C26" s="33"/>
@@ -1651,10 +1711,10 @@
       <c r="H26" s="35"/>
       <c r="I26" s="35"/>
       <c r="J26" s="35"/>
-      <c r="K26" s="51"/>
+      <c r="K26" s="35"/>
       <c r="L26" s="51"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="44"/>
+      <c r="M26" s="51"/>
+      <c r="N26" s="43"/>
       <c r="O26" s="44"/>
       <c r="P26" s="44"/>
       <c r="Q26" s="44"/>
@@ -1662,19 +1722,20 @@
       <c r="S26" s="44"/>
       <c r="T26" s="44"/>
       <c r="U26" s="44"/>
-      <c r="V26" s="43"/>
-      <c r="W26" s="45"/>
-      <c r="X26" s="43"/>
-      <c r="Y26" s="44"/>
+      <c r="V26" s="44"/>
+      <c r="W26" s="43"/>
+      <c r="X26" s="45"/>
+      <c r="Y26" s="43"/>
       <c r="Z26" s="44"/>
-      <c r="AA26" s="46"/>
+      <c r="AA26" s="44"/>
       <c r="AB26" s="46"/>
-      <c r="AC26" s="47"/>
-      <c r="AD26" s="48"/>
+      <c r="AC26" s="46"/>
+      <c r="AD26" s="47"/>
       <c r="AE26" s="48"/>
-      <c r="AF26" s="49"/>
-    </row>
-    <row r="27" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF26" s="48"/>
+      <c r="AG26" s="49"/>
+    </row>
+    <row r="27" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A27" s="33"/>
       <c r="B27" s="33"/>
       <c r="C27" s="33"/>
@@ -1685,10 +1746,10 @@
       <c r="H27" s="35"/>
       <c r="I27" s="35"/>
       <c r="J27" s="35"/>
-      <c r="K27" s="51"/>
+      <c r="K27" s="35"/>
       <c r="L27" s="51"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="44"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="43"/>
       <c r="O27" s="44"/>
       <c r="P27" s="44"/>
       <c r="Q27" s="44"/>
@@ -1696,19 +1757,20 @@
       <c r="S27" s="44"/>
       <c r="T27" s="44"/>
       <c r="U27" s="44"/>
-      <c r="V27" s="43"/>
-      <c r="W27" s="45"/>
-      <c r="X27" s="43"/>
-      <c r="Y27" s="44"/>
+      <c r="V27" s="44"/>
+      <c r="W27" s="43"/>
+      <c r="X27" s="45"/>
+      <c r="Y27" s="43"/>
       <c r="Z27" s="44"/>
-      <c r="AA27" s="46"/>
+      <c r="AA27" s="44"/>
       <c r="AB27" s="46"/>
-      <c r="AC27" s="47"/>
-      <c r="AD27" s="48"/>
+      <c r="AC27" s="46"/>
+      <c r="AD27" s="47"/>
       <c r="AE27" s="48"/>
-      <c r="AF27" s="17"/>
-    </row>
-    <row r="28" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF27" s="48"/>
+      <c r="AG27" s="17"/>
+    </row>
+    <row r="28" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="33"/>
       <c r="B28" s="33"/>
       <c r="C28" s="33"/>
@@ -1719,10 +1781,10 @@
       <c r="H28" s="35"/>
       <c r="I28" s="35"/>
       <c r="J28" s="35"/>
-      <c r="K28" s="51"/>
+      <c r="K28" s="35"/>
       <c r="L28" s="51"/>
-      <c r="M28" s="43"/>
-      <c r="N28" s="44"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="43"/>
       <c r="O28" s="44"/>
       <c r="P28" s="44"/>
       <c r="Q28" s="44"/>
@@ -1730,19 +1792,20 @@
       <c r="S28" s="44"/>
       <c r="T28" s="44"/>
       <c r="U28" s="44"/>
-      <c r="V28" s="43"/>
-      <c r="W28" s="45"/>
-      <c r="X28" s="43"/>
-      <c r="Y28" s="44"/>
+      <c r="V28" s="44"/>
+      <c r="W28" s="43"/>
+      <c r="X28" s="45"/>
+      <c r="Y28" s="43"/>
       <c r="Z28" s="44"/>
-      <c r="AA28" s="46"/>
+      <c r="AA28" s="44"/>
       <c r="AB28" s="46"/>
-      <c r="AC28" s="47"/>
-      <c r="AD28" s="48"/>
+      <c r="AC28" s="46"/>
+      <c r="AD28" s="47"/>
       <c r="AE28" s="48"/>
-      <c r="AF28" s="17"/>
-    </row>
-    <row r="29" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF28" s="48"/>
+      <c r="AG28" s="17"/>
+    </row>
+    <row r="29" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A29" s="33"/>
       <c r="B29" s="33"/>
       <c r="C29" s="33"/>
@@ -1753,10 +1816,10 @@
       <c r="H29" s="35"/>
       <c r="I29" s="35"/>
       <c r="J29" s="35"/>
-      <c r="K29" s="51"/>
+      <c r="K29" s="35"/>
       <c r="L29" s="51"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="44"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="43"/>
       <c r="O29" s="44"/>
       <c r="P29" s="44"/>
       <c r="Q29" s="44"/>
@@ -1764,19 +1827,20 @@
       <c r="S29" s="44"/>
       <c r="T29" s="44"/>
       <c r="U29" s="44"/>
-      <c r="V29" s="43"/>
-      <c r="W29" s="45"/>
-      <c r="X29" s="43"/>
-      <c r="Y29" s="44"/>
+      <c r="V29" s="44"/>
+      <c r="W29" s="43"/>
+      <c r="X29" s="45"/>
+      <c r="Y29" s="43"/>
       <c r="Z29" s="44"/>
-      <c r="AA29" s="46"/>
+      <c r="AA29" s="44"/>
       <c r="AB29" s="46"/>
-      <c r="AC29" s="47"/>
-      <c r="AD29" s="48"/>
+      <c r="AC29" s="46"/>
+      <c r="AD29" s="47"/>
       <c r="AE29" s="48"/>
-      <c r="AF29" s="17"/>
-    </row>
-    <row r="30" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF29" s="48"/>
+      <c r="AG29" s="17"/>
+    </row>
+    <row r="30" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A30" s="33"/>
       <c r="B30" s="33"/>
       <c r="C30" s="33"/>
@@ -1787,10 +1851,10 @@
       <c r="H30" s="35"/>
       <c r="I30" s="35"/>
       <c r="J30" s="35"/>
-      <c r="K30" s="51"/>
+      <c r="K30" s="35"/>
       <c r="L30" s="51"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="44"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="43"/>
       <c r="O30" s="44"/>
       <c r="P30" s="44"/>
       <c r="Q30" s="44"/>
@@ -1798,19 +1862,20 @@
       <c r="S30" s="44"/>
       <c r="T30" s="44"/>
       <c r="U30" s="44"/>
-      <c r="V30" s="43"/>
-      <c r="W30" s="45"/>
-      <c r="X30" s="43"/>
-      <c r="Y30" s="44"/>
+      <c r="V30" s="44"/>
+      <c r="W30" s="43"/>
+      <c r="X30" s="45"/>
+      <c r="Y30" s="43"/>
       <c r="Z30" s="44"/>
-      <c r="AA30" s="46"/>
+      <c r="AA30" s="44"/>
       <c r="AB30" s="46"/>
-      <c r="AC30" s="47"/>
-      <c r="AD30" s="48"/>
+      <c r="AC30" s="46"/>
+      <c r="AD30" s="47"/>
       <c r="AE30" s="48"/>
-      <c r="AF30" s="17"/>
-    </row>
-    <row r="31" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF30" s="48"/>
+      <c r="AG30" s="17"/>
+    </row>
+    <row r="31" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A31" s="33"/>
       <c r="B31" s="33"/>
       <c r="C31" s="33"/>
@@ -1821,10 +1886,10 @@
       <c r="H31" s="35"/>
       <c r="I31" s="35"/>
       <c r="J31" s="35"/>
-      <c r="K31" s="51"/>
+      <c r="K31" s="35"/>
       <c r="L31" s="51"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="44"/>
+      <c r="M31" s="51"/>
+      <c r="N31" s="43"/>
       <c r="O31" s="44"/>
       <c r="P31" s="44"/>
       <c r="Q31" s="44"/>
@@ -1832,19 +1897,20 @@
       <c r="S31" s="44"/>
       <c r="T31" s="44"/>
       <c r="U31" s="44"/>
-      <c r="V31" s="43"/>
-      <c r="W31" s="45"/>
-      <c r="X31" s="43"/>
-      <c r="Y31" s="44"/>
+      <c r="V31" s="44"/>
+      <c r="W31" s="43"/>
+      <c r="X31" s="45"/>
+      <c r="Y31" s="43"/>
       <c r="Z31" s="44"/>
-      <c r="AA31" s="46"/>
+      <c r="AA31" s="44"/>
       <c r="AB31" s="46"/>
-      <c r="AC31" s="47"/>
-      <c r="AD31" s="48"/>
+      <c r="AC31" s="46"/>
+      <c r="AD31" s="47"/>
       <c r="AE31" s="48"/>
-      <c r="AF31" s="17"/>
-    </row>
-    <row r="32" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF31" s="48"/>
+      <c r="AG31" s="17"/>
+    </row>
+    <row r="32" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A32" s="33"/>
       <c r="B32" s="33"/>
       <c r="C32" s="33"/>
@@ -1855,10 +1921,10 @@
       <c r="H32" s="35"/>
       <c r="I32" s="35"/>
       <c r="J32" s="35"/>
-      <c r="K32" s="51"/>
+      <c r="K32" s="35"/>
       <c r="L32" s="51"/>
-      <c r="M32" s="43"/>
-      <c r="N32" s="44"/>
+      <c r="M32" s="51"/>
+      <c r="N32" s="43"/>
       <c r="O32" s="44"/>
       <c r="P32" s="44"/>
       <c r="Q32" s="44"/>
@@ -1866,19 +1932,20 @@
       <c r="S32" s="44"/>
       <c r="T32" s="44"/>
       <c r="U32" s="44"/>
-      <c r="V32" s="43"/>
-      <c r="W32" s="45"/>
-      <c r="X32" s="43"/>
-      <c r="Y32" s="44"/>
+      <c r="V32" s="44"/>
+      <c r="W32" s="43"/>
+      <c r="X32" s="45"/>
+      <c r="Y32" s="43"/>
       <c r="Z32" s="44"/>
-      <c r="AA32" s="46"/>
+      <c r="AA32" s="44"/>
       <c r="AB32" s="46"/>
-      <c r="AC32" s="47"/>
-      <c r="AD32" s="48"/>
+      <c r="AC32" s="46"/>
+      <c r="AD32" s="47"/>
       <c r="AE32" s="48"/>
-      <c r="AF32" s="17"/>
-    </row>
-    <row r="33" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF32" s="48"/>
+      <c r="AG32" s="17"/>
+    </row>
+    <row r="33" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A33" s="33"/>
       <c r="B33" s="33"/>
       <c r="C33" s="33"/>
@@ -1889,10 +1956,10 @@
       <c r="H33" s="35"/>
       <c r="I33" s="35"/>
       <c r="J33" s="35"/>
-      <c r="K33" s="51"/>
+      <c r="K33" s="35"/>
       <c r="L33" s="51"/>
-      <c r="M33" s="43"/>
-      <c r="N33" s="44"/>
+      <c r="M33" s="51"/>
+      <c r="N33" s="43"/>
       <c r="O33" s="44"/>
       <c r="P33" s="44"/>
       <c r="Q33" s="44"/>
@@ -1900,19 +1967,20 @@
       <c r="S33" s="44"/>
       <c r="T33" s="44"/>
       <c r="U33" s="44"/>
-      <c r="V33" s="43"/>
-      <c r="W33" s="45"/>
-      <c r="X33" s="43"/>
-      <c r="Y33" s="44"/>
+      <c r="V33" s="44"/>
+      <c r="W33" s="43"/>
+      <c r="X33" s="45"/>
+      <c r="Y33" s="43"/>
       <c r="Z33" s="44"/>
-      <c r="AA33" s="46"/>
+      <c r="AA33" s="44"/>
       <c r="AB33" s="46"/>
-      <c r="AC33" s="47"/>
-      <c r="AD33" s="48"/>
+      <c r="AC33" s="46"/>
+      <c r="AD33" s="47"/>
       <c r="AE33" s="48"/>
-      <c r="AF33" s="17"/>
-    </row>
-    <row r="34" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF33" s="48"/>
+      <c r="AG33" s="17"/>
+    </row>
+    <row r="34" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A34" s="33"/>
       <c r="B34" s="33"/>
       <c r="C34" s="33"/>
@@ -1923,10 +1991,10 @@
       <c r="H34" s="35"/>
       <c r="I34" s="35"/>
       <c r="J34" s="35"/>
-      <c r="K34" s="51"/>
+      <c r="K34" s="35"/>
       <c r="L34" s="51"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="44"/>
+      <c r="M34" s="51"/>
+      <c r="N34" s="43"/>
       <c r="O34" s="44"/>
       <c r="P34" s="44"/>
       <c r="Q34" s="44"/>
@@ -1934,19 +2002,20 @@
       <c r="S34" s="44"/>
       <c r="T34" s="44"/>
       <c r="U34" s="44"/>
-      <c r="V34" s="43"/>
-      <c r="W34" s="45"/>
-      <c r="X34" s="43"/>
-      <c r="Y34" s="44"/>
+      <c r="V34" s="44"/>
+      <c r="W34" s="43"/>
+      <c r="X34" s="45"/>
+      <c r="Y34" s="43"/>
       <c r="Z34" s="44"/>
-      <c r="AA34" s="46"/>
+      <c r="AA34" s="44"/>
       <c r="AB34" s="46"/>
-      <c r="AC34" s="47"/>
-      <c r="AD34" s="48"/>
+      <c r="AC34" s="46"/>
+      <c r="AD34" s="47"/>
       <c r="AE34" s="48"/>
-      <c r="AF34" s="17"/>
-    </row>
-    <row r="35" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF34" s="48"/>
+      <c r="AG34" s="17"/>
+    </row>
+    <row r="35" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A35" s="33"/>
       <c r="B35" s="33"/>
       <c r="C35" s="33"/>
@@ -1957,10 +2026,10 @@
       <c r="H35" s="35"/>
       <c r="I35" s="35"/>
       <c r="J35" s="35"/>
-      <c r="K35" s="51"/>
+      <c r="K35" s="35"/>
       <c r="L35" s="51"/>
-      <c r="M35" s="43"/>
-      <c r="N35" s="44"/>
+      <c r="M35" s="51"/>
+      <c r="N35" s="43"/>
       <c r="O35" s="44"/>
       <c r="P35" s="44"/>
       <c r="Q35" s="44"/>
@@ -1968,19 +2037,20 @@
       <c r="S35" s="44"/>
       <c r="T35" s="44"/>
       <c r="U35" s="44"/>
-      <c r="V35" s="43"/>
-      <c r="W35" s="45"/>
-      <c r="X35" s="43"/>
-      <c r="Y35" s="44"/>
+      <c r="V35" s="44"/>
+      <c r="W35" s="43"/>
+      <c r="X35" s="45"/>
+      <c r="Y35" s="43"/>
       <c r="Z35" s="44"/>
-      <c r="AA35" s="46"/>
+      <c r="AA35" s="44"/>
       <c r="AB35" s="46"/>
-      <c r="AC35" s="47"/>
-      <c r="AD35" s="48"/>
+      <c r="AC35" s="46"/>
+      <c r="AD35" s="47"/>
       <c r="AE35" s="48"/>
-      <c r="AF35" s="17"/>
-    </row>
-    <row r="36" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF35" s="48"/>
+      <c r="AG35" s="17"/>
+    </row>
+    <row r="36" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A36" s="33"/>
       <c r="B36" s="33"/>
       <c r="C36" s="33"/>
@@ -1991,10 +2061,10 @@
       <c r="H36" s="35"/>
       <c r="I36" s="35"/>
       <c r="J36" s="35"/>
-      <c r="K36" s="51"/>
+      <c r="K36" s="35"/>
       <c r="L36" s="51"/>
-      <c r="M36" s="43"/>
-      <c r="N36" s="44"/>
+      <c r="M36" s="51"/>
+      <c r="N36" s="43"/>
       <c r="O36" s="44"/>
       <c r="P36" s="44"/>
       <c r="Q36" s="44"/>
@@ -2002,19 +2072,20 @@
       <c r="S36" s="44"/>
       <c r="T36" s="44"/>
       <c r="U36" s="44"/>
-      <c r="V36" s="43"/>
-      <c r="W36" s="45"/>
-      <c r="X36" s="43"/>
-      <c r="Y36" s="44"/>
+      <c r="V36" s="44"/>
+      <c r="W36" s="43"/>
+      <c r="X36" s="45"/>
+      <c r="Y36" s="43"/>
       <c r="Z36" s="44"/>
-      <c r="AA36" s="46"/>
+      <c r="AA36" s="44"/>
       <c r="AB36" s="46"/>
-      <c r="AC36" s="47"/>
-      <c r="AD36" s="48"/>
+      <c r="AC36" s="46"/>
+      <c r="AD36" s="47"/>
       <c r="AE36" s="48"/>
-      <c r="AF36" s="17"/>
-    </row>
-    <row r="37" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF36" s="48"/>
+      <c r="AG36" s="17"/>
+    </row>
+    <row r="37" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A37" s="33"/>
       <c r="B37" s="33"/>
       <c r="C37" s="33"/>
@@ -2025,10 +2096,10 @@
       <c r="H37" s="35"/>
       <c r="I37" s="35"/>
       <c r="J37" s="35"/>
-      <c r="K37" s="51"/>
+      <c r="K37" s="35"/>
       <c r="L37" s="51"/>
-      <c r="M37" s="43"/>
-      <c r="N37" s="44"/>
+      <c r="M37" s="51"/>
+      <c r="N37" s="43"/>
       <c r="O37" s="44"/>
       <c r="P37" s="44"/>
       <c r="Q37" s="44"/>
@@ -2036,19 +2107,20 @@
       <c r="S37" s="44"/>
       <c r="T37" s="44"/>
       <c r="U37" s="44"/>
-      <c r="V37" s="43"/>
-      <c r="W37" s="45"/>
-      <c r="X37" s="43"/>
-      <c r="Y37" s="44"/>
+      <c r="V37" s="44"/>
+      <c r="W37" s="43"/>
+      <c r="X37" s="45"/>
+      <c r="Y37" s="43"/>
       <c r="Z37" s="44"/>
-      <c r="AA37" s="46"/>
+      <c r="AA37" s="44"/>
       <c r="AB37" s="46"/>
-      <c r="AC37" s="47"/>
-      <c r="AD37" s="48"/>
+      <c r="AC37" s="46"/>
+      <c r="AD37" s="47"/>
       <c r="AE37" s="48"/>
-      <c r="AF37" s="49"/>
-    </row>
-    <row r="38" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF37" s="48"/>
+      <c r="AG37" s="49"/>
+    </row>
+    <row r="38" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A38" s="36"/>
       <c r="B38" s="36"/>
       <c r="C38" s="36"/>
@@ -2059,10 +2131,10 @@
       <c r="H38" s="37"/>
       <c r="I38" s="37"/>
       <c r="J38" s="37"/>
-      <c r="K38" s="13"/>
+      <c r="K38" s="37"/>
       <c r="L38" s="13"/>
-      <c r="M38" s="43"/>
-      <c r="N38" s="44"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="43"/>
       <c r="O38" s="44"/>
       <c r="P38" s="44"/>
       <c r="Q38" s="44"/>
@@ -2070,19 +2142,20 @@
       <c r="S38" s="44"/>
       <c r="T38" s="44"/>
       <c r="U38" s="44"/>
-      <c r="V38" s="43"/>
-      <c r="W38" s="45"/>
-      <c r="X38" s="43"/>
-      <c r="Y38" s="44"/>
+      <c r="V38" s="44"/>
+      <c r="W38" s="43"/>
+      <c r="X38" s="45"/>
+      <c r="Y38" s="43"/>
       <c r="Z38" s="44"/>
-      <c r="AA38" s="46"/>
+      <c r="AA38" s="44"/>
       <c r="AB38" s="46"/>
-      <c r="AC38" s="47"/>
-      <c r="AD38" s="48"/>
+      <c r="AC38" s="46"/>
+      <c r="AD38" s="47"/>
       <c r="AE38" s="48"/>
-      <c r="AF38" s="49"/>
-    </row>
-    <row r="39" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF38" s="48"/>
+      <c r="AG38" s="49"/>
+    </row>
+    <row r="39" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A39" s="33"/>
       <c r="B39" s="33"/>
       <c r="C39" s="33"/>
@@ -2093,10 +2166,10 @@
       <c r="H39" s="35"/>
       <c r="I39" s="35"/>
       <c r="J39" s="35"/>
-      <c r="K39" s="51"/>
+      <c r="K39" s="35"/>
       <c r="L39" s="51"/>
-      <c r="M39" s="43"/>
-      <c r="N39" s="44"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="43"/>
       <c r="O39" s="44"/>
       <c r="P39" s="44"/>
       <c r="Q39" s="44"/>
@@ -2104,19 +2177,20 @@
       <c r="S39" s="44"/>
       <c r="T39" s="44"/>
       <c r="U39" s="44"/>
-      <c r="V39" s="43"/>
-      <c r="W39" s="45"/>
-      <c r="X39" s="43"/>
-      <c r="Y39" s="44"/>
+      <c r="V39" s="44"/>
+      <c r="W39" s="43"/>
+      <c r="X39" s="45"/>
+      <c r="Y39" s="43"/>
       <c r="Z39" s="44"/>
-      <c r="AA39" s="46"/>
+      <c r="AA39" s="44"/>
       <c r="AB39" s="46"/>
-      <c r="AC39" s="47"/>
-      <c r="AD39" s="48"/>
+      <c r="AC39" s="46"/>
+      <c r="AD39" s="47"/>
       <c r="AE39" s="48"/>
-      <c r="AF39" s="49"/>
-    </row>
-    <row r="40" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF39" s="48"/>
+      <c r="AG39" s="49"/>
+    </row>
+    <row r="40" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A40" s="33"/>
       <c r="B40" s="33"/>
       <c r="C40" s="33"/>
@@ -2127,9 +2201,9 @@
       <c r="H40" s="35"/>
       <c r="I40" s="35"/>
       <c r="J40" s="35"/>
-      <c r="K40" s="51"/>
+      <c r="K40" s="35"/>
       <c r="L40" s="51"/>
-      <c r="M40" s="44"/>
+      <c r="M40" s="51"/>
       <c r="N40" s="44"/>
       <c r="O40" s="44"/>
       <c r="P40" s="44"/>
@@ -2138,19 +2212,20 @@
       <c r="S40" s="44"/>
       <c r="T40" s="44"/>
       <c r="U40" s="44"/>
-      <c r="V40" s="43"/>
-      <c r="W40" s="45"/>
-      <c r="X40" s="43"/>
-      <c r="Y40" s="44"/>
+      <c r="V40" s="44"/>
+      <c r="W40" s="43"/>
+      <c r="X40" s="45"/>
+      <c r="Y40" s="43"/>
       <c r="Z40" s="44"/>
-      <c r="AA40" s="46"/>
+      <c r="AA40" s="44"/>
       <c r="AB40" s="46"/>
-      <c r="AC40" s="47"/>
-      <c r="AD40" s="48"/>
+      <c r="AC40" s="46"/>
+      <c r="AD40" s="47"/>
       <c r="AE40" s="48"/>
-      <c r="AF40" s="49"/>
-    </row>
-    <row r="41" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF40" s="48"/>
+      <c r="AG40" s="49"/>
+    </row>
+    <row r="41" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A41" s="33"/>
       <c r="B41" s="33"/>
       <c r="C41" s="33"/>
@@ -2161,9 +2236,9 @@
       <c r="H41" s="35"/>
       <c r="I41" s="35"/>
       <c r="J41" s="35"/>
-      <c r="K41" s="51"/>
+      <c r="K41" s="35"/>
       <c r="L41" s="51"/>
-      <c r="M41" s="44"/>
+      <c r="M41" s="51"/>
       <c r="N41" s="44"/>
       <c r="O41" s="44"/>
       <c r="P41" s="44"/>
@@ -2172,19 +2247,20 @@
       <c r="S41" s="44"/>
       <c r="T41" s="44"/>
       <c r="U41" s="44"/>
-      <c r="V41" s="43"/>
-      <c r="W41" s="45"/>
-      <c r="X41" s="43"/>
-      <c r="Y41" s="44"/>
+      <c r="V41" s="44"/>
+      <c r="W41" s="43"/>
+      <c r="X41" s="45"/>
+      <c r="Y41" s="43"/>
       <c r="Z41" s="44"/>
-      <c r="AA41" s="46"/>
+      <c r="AA41" s="44"/>
       <c r="AB41" s="46"/>
-      <c r="AC41" s="47"/>
-      <c r="AD41" s="48"/>
+      <c r="AC41" s="46"/>
+      <c r="AD41" s="47"/>
       <c r="AE41" s="48"/>
-      <c r="AF41" s="49"/>
-    </row>
-    <row r="42" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF41" s="48"/>
+      <c r="AG41" s="49"/>
+    </row>
+    <row r="42" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A42" s="33"/>
       <c r="B42" s="33"/>
       <c r="C42" s="33"/>
@@ -2195,9 +2271,9 @@
       <c r="H42" s="35"/>
       <c r="I42" s="35"/>
       <c r="J42" s="35"/>
-      <c r="K42" s="51"/>
+      <c r="K42" s="35"/>
       <c r="L42" s="51"/>
-      <c r="M42" s="44"/>
+      <c r="M42" s="51"/>
       <c r="N42" s="44"/>
       <c r="O42" s="44"/>
       <c r="P42" s="44"/>
@@ -2206,19 +2282,20 @@
       <c r="S42" s="44"/>
       <c r="T42" s="44"/>
       <c r="U42" s="44"/>
-      <c r="V42" s="43"/>
-      <c r="W42" s="45"/>
-      <c r="X42" s="43"/>
-      <c r="Y42" s="44"/>
+      <c r="V42" s="44"/>
+      <c r="W42" s="43"/>
+      <c r="X42" s="45"/>
+      <c r="Y42" s="43"/>
       <c r="Z42" s="44"/>
-      <c r="AA42" s="46"/>
+      <c r="AA42" s="44"/>
       <c r="AB42" s="46"/>
-      <c r="AC42" s="47"/>
-      <c r="AD42" s="48"/>
+      <c r="AC42" s="46"/>
+      <c r="AD42" s="47"/>
       <c r="AE42" s="48"/>
-      <c r="AF42" s="49"/>
-    </row>
-    <row r="43" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF42" s="48"/>
+      <c r="AG42" s="49"/>
+    </row>
+    <row r="43" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A43" s="33"/>
       <c r="B43" s="33"/>
       <c r="C43" s="33"/>
@@ -2229,9 +2306,9 @@
       <c r="H43" s="35"/>
       <c r="I43" s="35"/>
       <c r="J43" s="35"/>
-      <c r="K43" s="51"/>
+      <c r="K43" s="35"/>
       <c r="L43" s="51"/>
-      <c r="M43" s="44"/>
+      <c r="M43" s="51"/>
       <c r="N43" s="44"/>
       <c r="O43" s="44"/>
       <c r="P43" s="44"/>
@@ -2240,19 +2317,20 @@
       <c r="S43" s="44"/>
       <c r="T43" s="44"/>
       <c r="U43" s="44"/>
-      <c r="V43" s="43"/>
-      <c r="W43" s="45"/>
-      <c r="X43" s="43"/>
-      <c r="Y43" s="44"/>
+      <c r="V43" s="44"/>
+      <c r="W43" s="43"/>
+      <c r="X43" s="45"/>
+      <c r="Y43" s="43"/>
       <c r="Z43" s="44"/>
-      <c r="AA43" s="46"/>
+      <c r="AA43" s="44"/>
       <c r="AB43" s="46"/>
-      <c r="AC43" s="47"/>
-      <c r="AD43" s="48"/>
+      <c r="AC43" s="46"/>
+      <c r="AD43" s="47"/>
       <c r="AE43" s="48"/>
-      <c r="AF43" s="49"/>
-    </row>
-    <row r="44" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF43" s="48"/>
+      <c r="AG43" s="49"/>
+    </row>
+    <row r="44" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="33"/>
@@ -2263,9 +2341,9 @@
       <c r="H44" s="35"/>
       <c r="I44" s="35"/>
       <c r="J44" s="35"/>
-      <c r="K44" s="51"/>
+      <c r="K44" s="35"/>
       <c r="L44" s="51"/>
-      <c r="M44" s="44"/>
+      <c r="M44" s="51"/>
       <c r="N44" s="44"/>
       <c r="O44" s="44"/>
       <c r="P44" s="44"/>
@@ -2274,19 +2352,20 @@
       <c r="S44" s="44"/>
       <c r="T44" s="44"/>
       <c r="U44" s="44"/>
-      <c r="V44" s="43"/>
-      <c r="W44" s="45"/>
-      <c r="X44" s="43"/>
-      <c r="Y44" s="44"/>
+      <c r="V44" s="44"/>
+      <c r="W44" s="43"/>
+      <c r="X44" s="45"/>
+      <c r="Y44" s="43"/>
       <c r="Z44" s="44"/>
-      <c r="AA44" s="46"/>
+      <c r="AA44" s="44"/>
       <c r="AB44" s="46"/>
-      <c r="AC44" s="47"/>
-      <c r="AD44" s="48"/>
+      <c r="AC44" s="46"/>
+      <c r="AD44" s="47"/>
       <c r="AE44" s="48"/>
-      <c r="AF44" s="49"/>
-    </row>
-    <row r="45" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF44" s="48"/>
+      <c r="AG44" s="49"/>
+    </row>
+    <row r="45" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="33"/>
@@ -2297,9 +2376,9 @@
       <c r="H45" s="35"/>
       <c r="I45" s="35"/>
       <c r="J45" s="35"/>
-      <c r="K45" s="51"/>
+      <c r="K45" s="35"/>
       <c r="L45" s="51"/>
-      <c r="M45" s="44"/>
+      <c r="M45" s="51"/>
       <c r="N45" s="44"/>
       <c r="O45" s="44"/>
       <c r="P45" s="44"/>
@@ -2308,19 +2387,20 @@
       <c r="S45" s="44"/>
       <c r="T45" s="44"/>
       <c r="U45" s="44"/>
-      <c r="V45" s="43"/>
-      <c r="W45" s="45"/>
-      <c r="X45" s="43"/>
-      <c r="Y45" s="44"/>
+      <c r="V45" s="44"/>
+      <c r="W45" s="43"/>
+      <c r="X45" s="45"/>
+      <c r="Y45" s="43"/>
       <c r="Z45" s="44"/>
-      <c r="AA45" s="46"/>
+      <c r="AA45" s="44"/>
       <c r="AB45" s="46"/>
-      <c r="AC45" s="47"/>
-      <c r="AD45" s="48"/>
+      <c r="AC45" s="46"/>
+      <c r="AD45" s="47"/>
       <c r="AE45" s="48"/>
-      <c r="AF45" s="49"/>
-    </row>
-    <row r="46" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF45" s="48"/>
+      <c r="AG45" s="49"/>
+    </row>
+    <row r="46" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A46" s="33"/>
       <c r="B46" s="33"/>
       <c r="C46" s="33"/>
@@ -2331,9 +2411,9 @@
       <c r="H46" s="35"/>
       <c r="I46" s="35"/>
       <c r="J46" s="35"/>
-      <c r="K46" s="51"/>
+      <c r="K46" s="35"/>
       <c r="L46" s="51"/>
-      <c r="M46" s="44"/>
+      <c r="M46" s="51"/>
       <c r="N46" s="44"/>
       <c r="O46" s="44"/>
       <c r="P46" s="44"/>
@@ -2342,19 +2422,20 @@
       <c r="S46" s="44"/>
       <c r="T46" s="44"/>
       <c r="U46" s="44"/>
-      <c r="V46" s="43"/>
-      <c r="W46" s="45"/>
-      <c r="X46" s="43"/>
-      <c r="Y46" s="44"/>
+      <c r="V46" s="44"/>
+      <c r="W46" s="43"/>
+      <c r="X46" s="45"/>
+      <c r="Y46" s="43"/>
       <c r="Z46" s="44"/>
-      <c r="AA46" s="46"/>
+      <c r="AA46" s="44"/>
       <c r="AB46" s="46"/>
-      <c r="AC46" s="47"/>
-      <c r="AD46" s="48"/>
+      <c r="AC46" s="46"/>
+      <c r="AD46" s="47"/>
       <c r="AE46" s="48"/>
-      <c r="AF46" s="49"/>
-    </row>
-    <row r="47" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF46" s="48"/>
+      <c r="AG46" s="49"/>
+    </row>
+    <row r="47" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A47" s="33"/>
       <c r="B47" s="33"/>
       <c r="C47" s="33"/>
@@ -2365,10 +2446,10 @@
       <c r="H47" s="35"/>
       <c r="I47" s="35"/>
       <c r="J47" s="35"/>
-      <c r="K47" s="51"/>
+      <c r="K47" s="35"/>
       <c r="L47" s="51"/>
-      <c r="M47" s="44"/>
-      <c r="N47" s="46"/>
+      <c r="M47" s="51"/>
+      <c r="N47" s="44"/>
       <c r="O47" s="46"/>
       <c r="P47" s="46"/>
       <c r="Q47" s="46"/>
@@ -2376,19 +2457,20 @@
       <c r="S47" s="46"/>
       <c r="T47" s="46"/>
       <c r="U47" s="46"/>
-      <c r="V47" s="48"/>
+      <c r="V47" s="46"/>
       <c r="W47" s="48"/>
-      <c r="X47" s="46"/>
+      <c r="X47" s="48"/>
       <c r="Y47" s="46"/>
       <c r="Z47" s="46"/>
       <c r="AA47" s="46"/>
       <c r="AB47" s="46"/>
-      <c r="AC47" s="47"/>
-      <c r="AD47" s="48"/>
+      <c r="AC47" s="46"/>
+      <c r="AD47" s="47"/>
       <c r="AE47" s="48"/>
-      <c r="AF47" s="49"/>
-    </row>
-    <row r="48" spans="1:32" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF47" s="48"/>
+      <c r="AG47" s="49"/>
+    </row>
+    <row r="48" spans="1:33" s="41" customFormat="1" ht="15" customHeight="1">
       <c r="A48" s="29"/>
       <c r="B48" s="29"/>
       <c r="C48" s="29"/>
@@ -2399,9 +2481,9 @@
       <c r="H48" s="15"/>
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
-      <c r="K48" s="39"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="46"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="39"/>
+      <c r="M48" s="15"/>
       <c r="N48" s="46"/>
       <c r="O48" s="46"/>
       <c r="P48" s="46"/>
@@ -2411,18 +2493,19 @@
       <c r="T48" s="46"/>
       <c r="U48" s="46"/>
       <c r="V48" s="46"/>
-      <c r="W48" s="48"/>
-      <c r="X48" s="46"/>
+      <c r="W48" s="46"/>
+      <c r="X48" s="48"/>
       <c r="Y48" s="46"/>
       <c r="Z48" s="46"/>
       <c r="AA48" s="46"/>
       <c r="AB48" s="46"/>
-      <c r="AC48" s="47"/>
-      <c r="AD48" s="48"/>
+      <c r="AC48" s="46"/>
+      <c r="AD48" s="47"/>
       <c r="AE48" s="48"/>
-      <c r="AF48" s="49"/>
-    </row>
-    <row r="49" spans="4:32" x14ac:dyDescent="0.2">
+      <c r="AF48" s="48"/>
+      <c r="AG48" s="49"/>
+    </row>
+    <row r="49" spans="4:33">
       <c r="D49" s="15"/>
       <c r="E49" s="15"/>
       <c r="F49" s="15"/>
@@ -2430,9 +2513,9 @@
       <c r="H49" s="15"/>
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
-      <c r="K49" s="39"/>
-      <c r="L49" s="15"/>
-      <c r="M49" s="46"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="39"/>
+      <c r="M49" s="15"/>
       <c r="N49" s="46"/>
       <c r="O49" s="46"/>
       <c r="P49" s="46"/>
@@ -2442,18 +2525,19 @@
       <c r="T49" s="46"/>
       <c r="U49" s="46"/>
       <c r="V49" s="46"/>
-      <c r="W49" s="48"/>
-      <c r="X49" s="46"/>
+      <c r="W49" s="46"/>
+      <c r="X49" s="48"/>
       <c r="Y49" s="46"/>
       <c r="Z49" s="46"/>
       <c r="AA49" s="46"/>
       <c r="AB49" s="46"/>
-      <c r="AC49" s="47"/>
-      <c r="AD49" s="48"/>
+      <c r="AC49" s="46"/>
+      <c r="AD49" s="47"/>
       <c r="AE49" s="48"/>
-      <c r="AF49" s="49"/>
-    </row>
-    <row r="50" spans="4:32" x14ac:dyDescent="0.2">
+      <c r="AF49" s="48"/>
+      <c r="AG49" s="49"/>
+    </row>
+    <row r="50" spans="4:33">
       <c r="D50" s="15"/>
       <c r="E50" s="15"/>
       <c r="F50" s="15"/>
@@ -2461,9 +2545,9 @@
       <c r="H50" s="15"/>
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
-      <c r="K50" s="39"/>
-      <c r="L50" s="15"/>
-      <c r="M50" s="46"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="39"/>
+      <c r="M50" s="15"/>
       <c r="N50" s="46"/>
       <c r="O50" s="46"/>
       <c r="P50" s="46"/>
@@ -2473,18 +2557,19 @@
       <c r="T50" s="46"/>
       <c r="U50" s="46"/>
       <c r="V50" s="46"/>
-      <c r="W50" s="48"/>
-      <c r="X50" s="46"/>
+      <c r="W50" s="46"/>
+      <c r="X50" s="48"/>
       <c r="Y50" s="46"/>
       <c r="Z50" s="46"/>
       <c r="AA50" s="46"/>
       <c r="AB50" s="46"/>
-      <c r="AC50" s="47"/>
-      <c r="AD50" s="48"/>
+      <c r="AC50" s="46"/>
+      <c r="AD50" s="47"/>
       <c r="AE50" s="48"/>
-      <c r="AF50" s="49"/>
-    </row>
-    <row r="51" spans="4:32" x14ac:dyDescent="0.2">
+      <c r="AF50" s="48"/>
+      <c r="AG50" s="49"/>
+    </row>
+    <row r="51" spans="4:33">
       <c r="D51" s="15"/>
       <c r="E51" s="15"/>
       <c r="F51" s="15"/>
@@ -2492,9 +2577,9 @@
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
-      <c r="K51" s="39"/>
-      <c r="L51" s="15"/>
-      <c r="M51" s="46"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="39"/>
+      <c r="M51" s="15"/>
       <c r="N51" s="46"/>
       <c r="O51" s="46"/>
       <c r="P51" s="46"/>
@@ -2504,18 +2589,19 @@
       <c r="T51" s="46"/>
       <c r="U51" s="46"/>
       <c r="V51" s="46"/>
-      <c r="W51" s="48"/>
-      <c r="X51" s="46"/>
+      <c r="W51" s="46"/>
+      <c r="X51" s="48"/>
       <c r="Y51" s="46"/>
       <c r="Z51" s="46"/>
       <c r="AA51" s="46"/>
       <c r="AB51" s="46"/>
-      <c r="AC51" s="47"/>
-      <c r="AD51" s="48"/>
+      <c r="AC51" s="46"/>
+      <c r="AD51" s="47"/>
       <c r="AE51" s="48"/>
-      <c r="AF51" s="49"/>
-    </row>
-    <row r="52" spans="4:32" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF51" s="48"/>
+      <c r="AG51" s="49"/>
+    </row>
+    <row r="52" spans="4:33" ht="15" customHeight="1">
       <c r="D52" s="15"/>
       <c r="E52" s="15"/>
       <c r="F52" s="15"/>
@@ -2523,10 +2609,10 @@
       <c r="H52" s="15"/>
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
-      <c r="K52" s="39"/>
-      <c r="L52" s="15"/>
-      <c r="M52" s="46"/>
-      <c r="N52" s="4"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="39"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="46"/>
       <c r="O52" s="4"/>
       <c r="P52" s="4"/>
       <c r="Q52" s="4"/>
@@ -2535,18 +2621,19 @@
       <c r="T52" s="4"/>
       <c r="U52" s="4"/>
       <c r="V52" s="4"/>
-      <c r="W52" s="6"/>
-      <c r="X52" s="4"/>
+      <c r="W52" s="4"/>
+      <c r="X52" s="6"/>
       <c r="Y52" s="4"/>
       <c r="Z52" s="4"/>
       <c r="AA52" s="4"/>
       <c r="AB52" s="4"/>
-      <c r="AC52" s="6"/>
+      <c r="AC52" s="4"/>
       <c r="AD52" s="6"/>
       <c r="AE52" s="6"/>
-      <c r="AF52" s="5"/>
-    </row>
-    <row r="53" spans="4:32" x14ac:dyDescent="0.2">
+      <c r="AF52" s="6"/>
+      <c r="AG52" s="5"/>
+    </row>
+    <row r="53" spans="4:33">
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
       <c r="F53" s="16"/>
@@ -2556,27 +2643,28 @@
       <c r="J53" s="16"/>
       <c r="K53" s="16"/>
       <c r="L53" s="16"/>
-      <c r="M53" s="4"/>
-    </row>
-    <row r="54" spans="4:32" x14ac:dyDescent="0.2">
-      <c r="W54" s="45"/>
-    </row>
-    <row r="56" spans="4:32" x14ac:dyDescent="0.2">
-      <c r="W56" s="8"/>
-    </row>
-    <row r="57" spans="4:32" x14ac:dyDescent="0.2">
-      <c r="W57" s="8"/>
-    </row>
-    <row r="58" spans="4:32" x14ac:dyDescent="0.2">
-      <c r="W58" s="8"/>
-    </row>
-    <row r="59" spans="4:32" x14ac:dyDescent="0.2">
-      <c r="W59" s="8"/>
+      <c r="M53" s="16"/>
+      <c r="N53" s="4"/>
+    </row>
+    <row r="54" spans="4:33">
+      <c r="X54" s="45"/>
+    </row>
+    <row r="56" spans="4:33">
+      <c r="X56" s="8"/>
+    </row>
+    <row r="57" spans="4:33">
+      <c r="X57" s="8"/>
+    </row>
+    <row r="58" spans="4:33">
+      <c r="X58" s="8"/>
+    </row>
+    <row r="59" spans="4:33">
+      <c r="X59" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2588,33 +2676,33 @@
       <selection activeCell="E34" sqref="A29:E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="4" max="4" width="6.25" style="27" customWidth="1"/>
     <col min="5" max="5" width="27.75" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="5:5" ht="17.25" customHeight="1">
       <c r="E1" s="44"/>
     </row>
-    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="17.25" customHeight="1">
       <c r="E23" s="44"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="D25" s="25"/>
       <c r="E25" s="24"/>
       <c r="I25" s="26"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="D26" s="25"/>
       <c r="E26" s="24"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="D27" s="25"/>
       <c r="E27" s="24"/>
       <c r="I27" s="26"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>66</v>
       </c>
@@ -2625,10 +2713,10 @@
         <v>134</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>59</v>
       </c>
@@ -2639,10 +2727,10 @@
         <v>128</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>37</v>
       </c>
@@ -2653,10 +2741,10 @@
         <v>89</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>5</v>
       </c>
@@ -2667,10 +2755,10 @@
         <v>45</v>
       </c>
       <c r="E32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>5</v>
       </c>
@@ -2681,10 +2769,10 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>11</v>
       </c>
@@ -2695,7 +2783,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>